<commit_message>
new class craeted for managing news and users
</commit_message>
<xml_diff>
--- a/7rmartFinalProject/src/test/resources/TestingData.xlsx
+++ b/7rmartFinalProject/src/test/resources/TestingData.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NITHYA R NAIR\eclipse-workspace\SuperMarket\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NITHYA R NAIR\git\7rMartFinalProject\7rmartFinalProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BC9E51-561A-4925-BBD8-3D83BCDF64BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A18C252-4781-48FF-981F-48A683A9E321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
+    <sheet name="AdminUserPage" sheetId="2" r:id="rId2"/>
+    <sheet name="ManageNewsPage" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,25 +27,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
   <si>
     <t>admin</t>
   </si>
   <si>
     <t>test</t>
   </si>
+  <si>
+    <t>testadminuser</t>
+  </si>
+  <si>
+    <t>testadminpassword</t>
+  </si>
+  <si>
+    <t>Political test issues</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,8 +83,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,7 +368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -391,4 +409,50 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F74070FB-07E2-432C-A8EE-757C992434A4}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.21875" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC9A578-0C1A-4405-90C0-C26AF1A2B1E6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>